<commit_message>
add alt explenation to the excel file
</commit_message>
<xml_diff>
--- a/Template-SEO-audit.xlsx
+++ b/Template-SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Bartek\Desktop\openclassrooms\P4_Bartosz_swiderski\Websites\P4-Project-Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61722428-89F6-4925-A52A-4D2929F2EA87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D80062-DB95-436D-8356-97063F4E78BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Category</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Hidden Keywords in page structure</t>
   </si>
   <si>
-    <t>adding hidden keywords is a black-hat technique to improve SEO, what could be easily recognized by SEO robots, if so, website could be penalized and not appearing in indexing. Also it might be affecting accessibility, since the keywords might be getting focus or be read by screen readers</t>
-  </si>
-  <si>
     <t>Never use any black-hat technices, it's a risky approach and might disable page indexing. Keep keywords in website content instead, maitaining it readable for user.</t>
   </si>
   <si>
@@ -127,6 +124,21 @@
   </si>
   <si>
     <t>Always adjust size of the images to their cointainer, use for that graphic applications instead of css</t>
+  </si>
+  <si>
+    <t>keywords in alt attribute in img elements</t>
+  </si>
+  <si>
+    <t>1. Alt attribute is meant to containt a short description of the content of the image, so screen readers can read them out for accessibillity purposes</t>
+  </si>
+  <si>
+    <t>2. Placing key words in alt attribute is a black hat technique, if found by SEO robots, website could be penalized and not appear in indexing</t>
+  </si>
+  <si>
+    <t>adding hidden keywords is a black-hat technique to improve SEO, what could be easily recognized by SEO robots, if so, website could be penalized and not appeari in indexing. Also it might be affecting accessibility, since the keywords might be getting focus or be read by screen readers</t>
+  </si>
+  <si>
+    <t>Always use short description of the content of each image on the website</t>
   </si>
 </sst>
 </file>
@@ -177,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -200,11 +212,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -218,6 +256,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -437,7 +484,7 @@
   <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -619,10 +666,10 @@
         <v>27</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="E9" s="4" t="b">
         <v>0</v>
@@ -631,37 +678,47 @@
     </row>
     <row r="10" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="C11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="E11" s="4" t="b">
         <v>0</v>
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+    <row r="12" spans="1:26" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="7"/>
       <c r="E12" s="4" t="b">
         <v>0</v>
       </c>
@@ -698,6 +755,11 @@
       <c r="F15" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>

<commit_message>
added v1 lighthouse reports & github links
</commit_message>
<xml_diff>
--- a/Template-SEO-audit.xlsx
+++ b/Template-SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Bartek\Desktop\openclassrooms\P4_Bartosz_swiderski\Websites\P4-Project-Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1E323E-ABE4-40F1-90AD-80BEFB2346AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5715F81-8749-4CAD-B3B9-648E3C1ECD1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="84">
   <si>
     <t>Category</t>
   </si>
@@ -133,12 +133,6 @@
   </si>
   <si>
     <t>https://www.w3schools.com/tags/att_global_lang.asp</t>
-  </si>
-  <si>
-    <t>Missing preloading request</t>
-  </si>
-  <si>
-    <t>https://web.dev/uses-rel-preload/?utm_source=lighthouse&amp;utm_medium=devtools</t>
   </si>
   <si>
     <t xml:space="preserve">https://web.dev/uses-webp-images/?utm_source=lighthouse&amp;utm_medium=devtools
@@ -281,19 +275,10 @@
     <t>Form elements do not have associated labels</t>
   </si>
   <si>
-    <t>Change rel=stylesheet to rel=preload for critical assets</t>
-  </si>
-  <si>
-    <t>Preloading critical assets could improve your website loading speed</t>
-  </si>
-  <si>
     <t>Always associate form elements with their labels</t>
   </si>
   <si>
     <t>Outline provides visual feedbacks to links and buttons on the website, it helps visual imparient users or those who don't use the mouse to navigate the website</t>
-  </si>
-  <si>
-    <t>W3C Validator</t>
   </si>
 </sst>
 </file>
@@ -363,7 +348,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,12 +359,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF7030A0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -411,7 +390,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -431,13 +410,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -655,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z24"/>
+  <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -720,7 +696,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F2" s="5"/>
     </row>
@@ -741,7 +717,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -752,7 +728,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>11</v>
@@ -761,7 +737,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -772,16 +748,16 @@
         <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E5" s="5" t="b">
         <v>0</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -795,13 +771,13 @@
         <v>14</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E6" s="5" t="b">
         <v>1</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -812,7 +788,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>16</v>
@@ -821,7 +797,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -829,10 +805,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>19</v>
@@ -852,7 +828,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>21</v>
@@ -861,7 +837,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -881,7 +857,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -889,53 +865,53 @@
         <v>22</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="E11" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>73</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="5" t="b">
         <v>0</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="9"/>
       <c r="E13" s="5" t="b">
         <v>0</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="47.25" x14ac:dyDescent="0.2">
@@ -943,7 +919,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>29</v>
@@ -955,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -963,19 +939,19 @@
         <v>22</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>77</v>
-      </c>
       <c r="E15" s="5" t="b">
         <v>0</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -983,13 +959,13 @@
         <v>22</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="E16" s="5" t="b">
         <v>0</v>
@@ -1009,7 +985,7 @@
         <v>32</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E17" s="7" t="b">
         <v>0</v>
@@ -1018,110 +994,88 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F18" s="9" t="s">
+    <row r="18" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="E18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="E19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>86</v>
+      <c r="D20" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="E20" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="F20" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="F20" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="63" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>57</v>
+      <c r="D21" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="E21" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="F21" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="63" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="5" t="s">
+      <c r="F21" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="2" t="s">
-        <v>88</v>
-      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>